<commit_message>
-added disclaimers in the top of the captial gains sheets of the Excel template file. -added adaptive treatment for case where the user has multiple accounts and the columns might shift -dealing with "mixed slash date formats" issue by assuming normal format first and switching if fails.
</commit_message>
<xml_diff>
--- a/tax_forms_template.xlsx
+++ b/tax_forms_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/talmiller/Dropbox/מסמכים/תיק השקעות/taxes/tax_forms_generator/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51B4F448-7132-594C-937C-566CE99D8D70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B0CE60C-584B-6244-9C12-E166A49F104A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16000" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dividends" sheetId="6" r:id="rId1"/>
@@ -1504,9 +1504,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{710AD44E-F847-6C41-BCA9-7538B986DE33}">
   <dimension ref="A1:AB204"/>
   <sheetViews>
-    <sheetView rightToLeft="1" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
-    </sheetView>
+    <sheetView rightToLeft="1" tabSelected="1" zoomScaleNormal="125" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -7168,7 +7166,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23CD7FF3-3014-E540-B371-93725F8A5AE7}">
   <dimension ref="B2:Z204"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" zoomScaleNormal="125" workbookViewId="0">
+    <sheetView rightToLeft="1" zoomScaleNormal="125" workbookViewId="0">
       <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>

</xml_diff>